<commit_message>
chore: updating dataset from new images
</commit_message>
<xml_diff>
--- a/data/Truth.xlsx
+++ b/data/Truth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\AI Projects\otter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3702C751-B401-4FB7-A278-2442FF5155A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90A6BFE-74C5-4080-9A6F-2B3B71F0D764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="0" windowWidth="24330" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28815" yWindow="0" windowWidth="17415" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Image</t>
   </si>
@@ -256,6 +256,30 @@
   </si>
   <si>
     <t>Possum</t>
+  </si>
+  <si>
+    <t>250313_KEN1_0</t>
+  </si>
+  <si>
+    <t>250314_KEN1_0</t>
+  </si>
+  <si>
+    <t>250317_BSHNL_0</t>
+  </si>
+  <si>
+    <t>250317_BSHNL_1</t>
+  </si>
+  <si>
+    <t>250317_BSHNL_2</t>
+  </si>
+  <si>
+    <t>250318_BOB_0</t>
+  </si>
+  <si>
+    <t>250318_BOB_1</t>
+  </si>
+  <si>
+    <t>250319_KEN1_0</t>
   </si>
 </sst>
 </file>
@@ -312,15 +336,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -603,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R62"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M62" sqref="M62"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,52 +651,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -699,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <f>SUM(E2:F2)</f>
+        <f t="shared" ref="G2:G33" si="0">SUM(E2:F2)</f>
         <v>2</v>
       </c>
       <c r="H2" s="1">
@@ -750,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="1">
-        <f>SUM(E3:F3)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H3" s="1">
@@ -801,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <f>SUM(E4:F4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="1">
@@ -852,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <f>SUM(E5:F5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H5" s="1">
@@ -903,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <f>SUM(E6:F6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H6" s="1">
@@ -954,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="1">
-        <f>SUM(E7:F7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H7" s="1">
@@ -1005,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <f>SUM(E8:F8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8" s="1">
@@ -1056,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <f>SUM(E9:F9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H9" s="1">
@@ -1107,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <f>SUM(E10:F10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H10" s="1">
@@ -1158,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="1">
-        <f>SUM(E11:F11)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H11" s="1">
@@ -1209,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <f>SUM(E12:F12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H12" s="1">
@@ -1262,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <f>SUM(E13:F13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H13" s="1">
@@ -1313,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <f>SUM(E14:F14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="1">
@@ -1364,7 +1385,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="1">
-        <f>SUM(E15:F15)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H15" s="1">
@@ -1415,7 +1436,7 @@
         <v>13</v>
       </c>
       <c r="G16" s="1">
-        <f>SUM(E16:F16)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="H16" s="1">
@@ -1466,7 +1487,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <f>SUM(E17:F17)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H17" s="1">
@@ -1517,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="1">
-        <f>SUM(E18:F18)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H18" s="1">
@@ -1568,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="1">
-        <f>SUM(E19:F19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H19" s="1">
@@ -1619,7 +1640,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="1">
-        <f>SUM(E20:F20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" s="1">
@@ -1670,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <f>SUM(E21:F21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" s="1">
@@ -1721,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="1">
-        <f>SUM(E22:F22)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H22" s="1">
@@ -1772,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="1">
-        <f>SUM(E23:F23)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H23" s="1">
@@ -1823,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="1">
-        <f>SUM(E24:F24)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H24" s="1">
@@ -1874,7 +1895,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="1">
-        <f>SUM(E25:F25)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H25" s="1">
@@ -1925,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="1">
-        <f>SUM(E26:F26)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H26" s="1">
@@ -1976,7 +1997,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <f>SUM(E27:F27)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H27" s="1">
@@ -2027,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="1">
-        <f>SUM(E28:F28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H28" s="1">
@@ -2078,7 +2099,7 @@
         <v>13</v>
       </c>
       <c r="G29" s="1">
-        <f>SUM(E29:F29)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="H29" s="1">
@@ -2129,7 +2150,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="1">
-        <f>SUM(E30:F30)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H30" s="1">
@@ -2180,7 +2201,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="1">
-        <f>SUM(E31:F31)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H31" s="1">
@@ -2231,7 +2252,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="1">
-        <f>SUM(E32:F32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H32" s="1">
@@ -2282,7 +2303,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="1">
-        <f>SUM(E33:F33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H33" s="1">
@@ -2333,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="1">
-        <f>SUM(E34:F34)</f>
+        <f t="shared" ref="G34:G86" si="1">SUM(E34:F34)</f>
         <v>0</v>
       </c>
       <c r="H34" s="1">
@@ -2384,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="1">
-        <f>SUM(E35:F35)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H35" s="1">
@@ -2435,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="1">
-        <f>SUM(E36:F36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H36" s="1">
@@ -2486,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="1">
-        <f>SUM(E37:F37)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H37" s="1">
@@ -2537,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="1">
-        <f>SUM(E38:F38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H38" s="1">
@@ -2588,7 +2609,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="1">
-        <f>SUM(E39:F39)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H39" s="1">
@@ -2639,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="1">
-        <f>SUM(E40:F40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H40" s="1">
@@ -2690,7 +2711,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="1">
-        <f>SUM(E41:F41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H41" s="1">
@@ -2741,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="1">
-        <f>SUM(E42:F42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H42" s="1">
@@ -2792,7 +2813,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="1">
-        <f>SUM(E43:F43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H43" s="1">
@@ -2843,7 +2864,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="1">
-        <f>SUM(E44:F44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H44" s="1">
@@ -2894,7 +2915,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="1">
-        <f>SUM(E45:F45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H45" s="1">
@@ -2945,7 +2966,7 @@
         <v>3</v>
       </c>
       <c r="G46" s="1">
-        <f>SUM(E46:F46)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H46" s="1">
@@ -2996,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="1">
-        <f>SUM(E47:F47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H47" s="1">
@@ -3047,7 +3068,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="1">
-        <f>SUM(E48:F48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H48" s="1">
@@ -3098,7 +3119,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="1">
-        <f>SUM(E49:F49)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H49" s="1">
@@ -3149,7 +3170,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="1">
-        <f>SUM(E50:F50)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H50" s="1">
@@ -3180,7 +3201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
@@ -3200,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="1">
-        <f>SUM(E51:F51)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H51" s="1">
@@ -3231,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -3251,7 +3272,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="1">
-        <f>SUM(E52:F52)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H52" s="1">
@@ -3282,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
@@ -3302,7 +3323,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="1">
-        <f>SUM(E53:F53)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H53" s="1">
@@ -3333,7 +3354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
@@ -3353,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="G54" s="1">
-        <f>SUM(E54:F54)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H54" s="1">
@@ -3384,7 +3405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
@@ -3404,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="1">
-        <f>SUM(E55:F55)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H55" s="1">
@@ -3435,7 +3456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
@@ -3455,7 +3476,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="1">
-        <f>SUM(E56:F56)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H56" s="1">
@@ -3486,109 +3507,109 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B57" s="1">
         <v>2025</v>
       </c>
-      <c r="C57" s="2">
-        <v>3</v>
-      </c>
-      <c r="D57" s="2">
+      <c r="C57" s="1">
+        <v>3</v>
+      </c>
+      <c r="D57" s="1">
         <v>7</v>
       </c>
-      <c r="E57" s="2">
-        <v>1</v>
-      </c>
-      <c r="F57" s="2">
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
         <v>1</v>
       </c>
       <c r="G57" s="1">
-        <f>SUM(E57:F57)</f>
-        <v>2</v>
-      </c>
-      <c r="H57" s="2">
-        <v>0</v>
-      </c>
-      <c r="I57" s="2">
-        <v>0</v>
-      </c>
-      <c r="J57" s="2">
-        <v>0</v>
-      </c>
-      <c r="K57" s="2">
-        <v>0</v>
-      </c>
-      <c r="L57" s="2">
-        <v>0</v>
-      </c>
-      <c r="M57" s="2">
-        <v>0</v>
-      </c>
-      <c r="N57" s="2">
-        <v>0</v>
-      </c>
-      <c r="O57" s="2">
-        <v>0</v>
-      </c>
-      <c r="P57" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0</v>
+      </c>
+      <c r="K57" s="1">
+        <v>0</v>
+      </c>
+      <c r="L57" s="1">
+        <v>0</v>
+      </c>
+      <c r="M57" s="1">
+        <v>0</v>
+      </c>
+      <c r="N57" s="1">
+        <v>0</v>
+      </c>
+      <c r="O57" s="1">
+        <v>0</v>
+      </c>
+      <c r="P57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B58" s="1">
         <v>2025</v>
       </c>
-      <c r="C58" s="2">
-        <v>3</v>
-      </c>
-      <c r="D58" s="2">
+      <c r="C58" s="1">
+        <v>3</v>
+      </c>
+      <c r="D58" s="1">
         <v>7</v>
       </c>
-      <c r="E58" s="2">
-        <v>0</v>
-      </c>
-      <c r="F58" s="2">
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
         <v>0</v>
       </c>
       <c r="G58" s="1">
-        <f>SUM(E58:F58)</f>
-        <v>0</v>
-      </c>
-      <c r="H58" s="2">
-        <v>0</v>
-      </c>
-      <c r="I58" s="2">
-        <v>0</v>
-      </c>
-      <c r="J58" s="2">
-        <v>0</v>
-      </c>
-      <c r="K58" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0</v>
+      </c>
+      <c r="K58" s="1">
         <v>8</v>
       </c>
-      <c r="L58" s="2">
-        <v>0</v>
-      </c>
-      <c r="M58" s="2">
-        <v>0</v>
-      </c>
-      <c r="N58" s="2">
-        <v>0</v>
-      </c>
-      <c r="O58" s="2">
-        <v>0</v>
-      </c>
-      <c r="P58" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L58" s="1">
+        <v>0</v>
+      </c>
+      <c r="M58" s="1">
+        <v>0</v>
+      </c>
+      <c r="N58" s="1">
+        <v>0</v>
+      </c>
+      <c r="O58" s="1">
+        <v>0</v>
+      </c>
+      <c r="P58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>51</v>
       </c>
@@ -3608,7 +3629,7 @@
         <v>0</v>
       </c>
       <c r="G59" s="1">
-        <f>SUM(E59:F59)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H59" s="1">
@@ -3639,156 +3660,566 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B60" s="1">
         <v>2025</v>
       </c>
-      <c r="C60" s="2">
-        <v>3</v>
-      </c>
-      <c r="D60" s="2">
+      <c r="C60" s="1">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1">
         <v>8</v>
       </c>
-      <c r="E60" s="2">
-        <v>0</v>
-      </c>
-      <c r="F60" s="2">
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
         <v>0</v>
       </c>
       <c r="G60" s="1">
-        <f>SUM(E60:F60)</f>
-        <v>0</v>
-      </c>
-      <c r="H60" s="2">
-        <v>0</v>
-      </c>
-      <c r="I60" s="2">
-        <v>0</v>
-      </c>
-      <c r="J60" s="2">
-        <v>2</v>
-      </c>
-      <c r="K60" s="2">
-        <v>0</v>
-      </c>
-      <c r="L60" s="2">
-        <v>0</v>
-      </c>
-      <c r="M60" s="2">
-        <v>0</v>
-      </c>
-      <c r="N60" s="2">
-        <v>1</v>
-      </c>
-      <c r="O60" s="2">
-        <v>0</v>
-      </c>
-      <c r="P60" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0</v>
+      </c>
+      <c r="J60" s="1">
+        <v>2</v>
+      </c>
+      <c r="K60" s="1">
+        <v>0</v>
+      </c>
+      <c r="L60" s="1">
+        <v>0</v>
+      </c>
+      <c r="M60" s="1">
+        <v>0</v>
+      </c>
+      <c r="N60" s="1">
+        <v>1</v>
+      </c>
+      <c r="O60" s="1">
+        <v>0</v>
+      </c>
+      <c r="P60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B61" s="1">
         <v>2025</v>
       </c>
-      <c r="C61" s="2">
-        <v>3</v>
-      </c>
-      <c r="D61" s="2">
+      <c r="C61" s="1">
+        <v>3</v>
+      </c>
+      <c r="D61" s="1">
         <v>10</v>
       </c>
-      <c r="E61" s="2">
-        <v>0</v>
-      </c>
-      <c r="F61" s="2">
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
         <v>0</v>
       </c>
       <c r="G61" s="1">
-        <f>SUM(E61:F61)</f>
-        <v>0</v>
-      </c>
-      <c r="H61" s="2">
-        <v>0</v>
-      </c>
-      <c r="I61" s="2">
-        <v>0</v>
-      </c>
-      <c r="J61" s="2">
-        <v>0</v>
-      </c>
-      <c r="K61" s="2">
-        <v>2</v>
-      </c>
-      <c r="L61" s="2">
-        <v>0</v>
-      </c>
-      <c r="M61" s="2">
-        <v>0</v>
-      </c>
-      <c r="N61" s="2">
-        <v>0</v>
-      </c>
-      <c r="O61" s="2">
-        <v>0</v>
-      </c>
-      <c r="P61" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0</v>
+      </c>
+      <c r="K61" s="1">
+        <v>2</v>
+      </c>
+      <c r="L61" s="1">
+        <v>0</v>
+      </c>
+      <c r="M61" s="1">
+        <v>0</v>
+      </c>
+      <c r="N61" s="1">
+        <v>0</v>
+      </c>
+      <c r="O61" s="1">
+        <v>0</v>
+      </c>
+      <c r="P61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B62" s="1">
         <v>2025</v>
       </c>
-      <c r="C62" s="2">
-        <v>3</v>
-      </c>
-      <c r="D62" s="2">
+      <c r="C62" s="1">
+        <v>3</v>
+      </c>
+      <c r="D62" s="1">
         <v>10</v>
       </c>
-      <c r="E62" s="2">
-        <v>0</v>
-      </c>
-      <c r="F62" s="2">
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
         <v>0</v>
       </c>
       <c r="G62" s="1">
-        <f>SUM(E62:F62)</f>
-        <v>0</v>
-      </c>
-      <c r="H62" s="2">
-        <v>0</v>
-      </c>
-      <c r="I62" s="2">
-        <v>0</v>
-      </c>
-      <c r="J62" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0</v>
+      </c>
+      <c r="J62" s="1">
         <v>6</v>
       </c>
-      <c r="K62" s="2">
-        <v>0</v>
-      </c>
-      <c r="L62" s="2">
-        <v>0</v>
-      </c>
-      <c r="M62" s="2">
-        <v>0</v>
-      </c>
-      <c r="N62" s="2">
-        <v>0</v>
-      </c>
-      <c r="O62" s="2">
-        <v>0</v>
-      </c>
-      <c r="P62" s="2">
+      <c r="K62" s="1">
+        <v>0</v>
+      </c>
+      <c r="L62" s="1">
+        <v>0</v>
+      </c>
+      <c r="M62" s="1">
+        <v>0</v>
+      </c>
+      <c r="N62" s="1">
+        <v>0</v>
+      </c>
+      <c r="O62" s="1">
+        <v>0</v>
+      </c>
+      <c r="P62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C63" s="1">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1">
+        <v>13</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0</v>
+      </c>
+      <c r="J63" s="1">
+        <v>2</v>
+      </c>
+      <c r="K63" s="1">
+        <v>0</v>
+      </c>
+      <c r="L63" s="1">
+        <v>0</v>
+      </c>
+      <c r="M63" s="1">
+        <v>0</v>
+      </c>
+      <c r="N63" s="1">
+        <v>0</v>
+      </c>
+      <c r="O63" s="1">
+        <v>0</v>
+      </c>
+      <c r="P63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C64" s="1">
+        <v>3</v>
+      </c>
+      <c r="D64" s="1">
+        <v>14</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="1">
+        <v>15</v>
+      </c>
+      <c r="K64" s="1">
+        <v>0</v>
+      </c>
+      <c r="L64" s="1">
+        <v>0</v>
+      </c>
+      <c r="M64" s="1">
+        <v>0</v>
+      </c>
+      <c r="N64" s="1">
+        <v>0</v>
+      </c>
+      <c r="O64" s="1">
+        <v>0</v>
+      </c>
+      <c r="P64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C65" s="1">
+        <v>3</v>
+      </c>
+      <c r="D65" s="1">
+        <v>17</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0</v>
+      </c>
+      <c r="J65" s="1">
+        <v>25</v>
+      </c>
+      <c r="K65" s="1">
+        <v>0</v>
+      </c>
+      <c r="L65" s="1">
+        <v>0</v>
+      </c>
+      <c r="M65" s="1">
+        <v>0</v>
+      </c>
+      <c r="N65" s="1">
+        <v>0</v>
+      </c>
+      <c r="O65" s="1">
+        <v>0</v>
+      </c>
+      <c r="P65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C66" s="1">
+        <v>3</v>
+      </c>
+      <c r="D66" s="1">
+        <v>17</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H66" s="1">
+        <v>0</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0</v>
+      </c>
+      <c r="J66" s="1">
+        <v>9</v>
+      </c>
+      <c r="K66" s="1">
+        <v>0</v>
+      </c>
+      <c r="L66" s="1">
+        <v>0</v>
+      </c>
+      <c r="M66" s="1">
+        <v>0</v>
+      </c>
+      <c r="N66" s="1">
+        <v>0</v>
+      </c>
+      <c r="O66" s="1">
+        <v>0</v>
+      </c>
+      <c r="P66" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="1"/>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C67" s="1">
+        <v>3</v>
+      </c>
+      <c r="D67" s="1">
+        <v>17</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0</v>
+      </c>
+      <c r="F67" s="1">
+        <v>0</v>
+      </c>
+      <c r="G67" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H67" s="1">
+        <v>0</v>
+      </c>
+      <c r="I67" s="1">
+        <v>0</v>
+      </c>
+      <c r="J67" s="1">
+        <v>5</v>
+      </c>
+      <c r="K67" s="1">
+        <v>0</v>
+      </c>
+      <c r="L67" s="1">
+        <v>0</v>
+      </c>
+      <c r="M67" s="1">
+        <v>0</v>
+      </c>
+      <c r="N67" s="1">
+        <v>0</v>
+      </c>
+      <c r="O67" s="1">
+        <v>0</v>
+      </c>
+      <c r="P67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B68" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C68" s="1">
+        <v>3</v>
+      </c>
+      <c r="D68" s="1">
+        <v>18</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0</v>
+      </c>
+      <c r="F68" s="1">
+        <v>2</v>
+      </c>
+      <c r="G68" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0</v>
+      </c>
+      <c r="J68" s="1">
+        <v>0</v>
+      </c>
+      <c r="K68" s="1">
+        <v>2</v>
+      </c>
+      <c r="L68" s="1">
+        <v>0</v>
+      </c>
+      <c r="M68" s="1">
+        <v>0</v>
+      </c>
+      <c r="N68" s="1">
+        <v>0</v>
+      </c>
+      <c r="O68" s="1">
+        <v>0</v>
+      </c>
+      <c r="P68" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="1"/>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C69" s="1">
+        <v>3</v>
+      </c>
+      <c r="D69" s="1">
+        <v>18</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0</v>
+      </c>
+      <c r="G69" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0</v>
+      </c>
+      <c r="J69" s="1">
+        <v>17</v>
+      </c>
+      <c r="K69" s="1">
+        <v>0</v>
+      </c>
+      <c r="L69" s="1">
+        <v>0</v>
+      </c>
+      <c r="M69" s="1">
+        <v>0</v>
+      </c>
+      <c r="N69" s="1">
+        <v>0</v>
+      </c>
+      <c r="O69" s="1">
+        <v>0</v>
+      </c>
+      <c r="P69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C70" s="1">
+        <v>3</v>
+      </c>
+      <c r="D70" s="1">
+        <v>19</v>
+      </c>
+      <c r="E70" s="1">
+        <v>0</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0</v>
+      </c>
+      <c r="J70" s="1">
+        <v>7</v>
+      </c>
+      <c r="K70" s="1">
+        <v>0</v>
+      </c>
+      <c r="L70" s="1">
+        <v>0</v>
+      </c>
+      <c r="M70" s="1">
+        <v>0</v>
+      </c>
+      <c r="N70" s="1">
+        <v>0</v>
+      </c>
+      <c r="O70" s="1">
+        <v>0</v>
+      </c>
+      <c r="P70" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: adding data, updating truth values
</commit_message>
<xml_diff>
--- a/data/Truth.xlsx
+++ b/data/Truth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\AI Projects\otter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90A6BFE-74C5-4080-9A6F-2B3B71F0D764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2344B6B-AB90-4973-8F5C-3478325AD4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28815" yWindow="0" windowWidth="17415" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28815" yWindow="75" windowWidth="24330" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Image</t>
   </si>
@@ -280,6 +280,21 @@
   </si>
   <si>
     <t>250319_KEN1_0</t>
+  </si>
+  <si>
+    <t>250324_BSHNL_0</t>
+  </si>
+  <si>
+    <t>250324_BSHNL_1</t>
+  </si>
+  <si>
+    <t>250324_BSHNL_2</t>
+  </si>
+  <si>
+    <t>241122_TRLCAM_0</t>
+  </si>
+  <si>
+    <t>Eagle</t>
   </si>
 </sst>
 </file>
@@ -624,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R70"/>
+  <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,6 +714,9 @@
       <c r="P1" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="Q1" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -720,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <f t="shared" ref="G2:G33" si="0">SUM(E2:F2)</f>
+        <f t="shared" ref="G2:G34" si="0">SUM(E2:F2)</f>
         <v>2</v>
       </c>
       <c r="H2" s="1">
@@ -748,6 +766,9 @@
         <v>0</v>
       </c>
       <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
         <v>0</v>
       </c>
     </row>
@@ -801,6 +822,9 @@
       <c r="P3" s="1">
         <v>0</v>
       </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -852,6 +876,9 @@
       <c r="P4" s="1">
         <v>0</v>
       </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -903,6 +930,9 @@
       <c r="P5" s="1">
         <v>0</v>
       </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -954,6 +984,9 @@
       <c r="P6" s="1">
         <v>0</v>
       </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1005,6 +1038,9 @@
       <c r="P7" s="1">
         <v>0</v>
       </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1056,6 +1092,9 @@
       <c r="P8" s="1">
         <v>0</v>
       </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1107,29 +1146,32 @@
       <c r="P9" s="1">
         <v>0</v>
       </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="B10" s="1">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
@@ -1147,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N10" s="1">
         <v>0</v>
@@ -1157,11 +1199,14 @@
       </c>
       <c r="P10" s="1">
         <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>2025</v>
@@ -1173,14 +1218,14 @@
         <v>17</v>
       </c>
       <c r="E11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
@@ -1207,12 +1252,15 @@
         <v>0</v>
       </c>
       <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
         <v>2025</v>
@@ -1221,17 +1269,17 @@
         <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
@@ -1260,12 +1308,13 @@
       <c r="P12" s="1">
         <v>0</v>
       </c>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
         <v>2025</v>
@@ -1313,10 +1362,14 @@
       <c r="P13" s="1">
         <v>0</v>
       </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1">
         <v>2025</v>
@@ -1328,14 +1381,14 @@
         <v>18</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
@@ -1350,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1">
         <v>0</v>
@@ -1362,12 +1415,15 @@
         <v>0</v>
       </c>
       <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1">
         <v>2025</v>
@@ -1376,17 +1432,17 @@
         <v>1</v>
       </c>
       <c r="D15" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E15" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
@@ -1401,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="1">
         <v>0</v>
@@ -1413,12 +1469,15 @@
         <v>0</v>
       </c>
       <c r="P15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
         <v>2025</v>
@@ -1427,68 +1486,71 @@
         <v>1</v>
       </c>
       <c r="D16" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>24</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
         <v>13</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
-        <v>0</v>
-      </c>
-      <c r="L16" s="1">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1">
-        <v>0</v>
-      </c>
-      <c r="P16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1">
-        <v>5</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -1517,10 +1579,13 @@
       <c r="P17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="1">
         <v>2025</v>
@@ -1529,17 +1594,17 @@
         <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -1568,10 +1633,13 @@
       <c r="P18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1">
         <v>2025</v>
@@ -1580,17 +1648,17 @@
         <v>2</v>
       </c>
       <c r="D19" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
@@ -1602,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
@@ -1619,10 +1687,13 @@
       <c r="P19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1">
         <v>2025</v>
@@ -1631,29 +1702,29 @@
         <v>2</v>
       </c>
       <c r="D20" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
       </c>
       <c r="I20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
@@ -1670,10 +1741,13 @@
       <c r="P20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="1">
         <v>2025</v>
@@ -1682,7 +1756,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -1695,10 +1769,10 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
@@ -1721,10 +1795,13 @@
       <c r="P21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1">
         <v>2025</v>
@@ -1733,20 +1810,20 @@
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E22" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="1">
         <v>0</v>
@@ -1772,10 +1849,13 @@
       <c r="P22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1">
         <v>2025</v>
@@ -1784,13 +1864,13 @@
         <v>2</v>
       </c>
       <c r="D23" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="0"/>
@@ -1803,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K23" s="1">
         <v>0</v>
@@ -1823,10 +1903,13 @@
       <c r="P23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B24" s="1">
         <v>2025</v>
@@ -1838,14 +1921,14 @@
         <v>14</v>
       </c>
       <c r="E24" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
@@ -1854,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K24" s="1">
         <v>0</v>
@@ -1874,10 +1957,13 @@
       <c r="P24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1">
         <v>2025</v>
@@ -1886,13 +1972,13 @@
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="0"/>
@@ -1905,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K25" s="1">
         <v>0</v>
@@ -1925,10 +2011,13 @@
       <c r="P25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1">
         <v>2025</v>
@@ -1937,17 +2026,17 @@
         <v>2</v>
       </c>
       <c r="D26" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
@@ -1956,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K26" s="1">
         <v>0</v>
@@ -1976,10 +2065,13 @@
       <c r="P26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1">
         <v>2025</v>
@@ -1988,17 +2080,17 @@
         <v>2</v>
       </c>
       <c r="D27" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E27" s="1">
         <v>2</v>
       </c>
       <c r="F27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H27" s="1">
         <v>0</v>
@@ -2027,10 +2119,13 @@
       <c r="P27" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>2025</v>
@@ -2042,14 +2137,14 @@
         <v>18</v>
       </c>
       <c r="E28" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" s="1">
         <v>0</v>
@@ -2078,10 +2173,13 @@
       <c r="P28" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1">
         <v>2025</v>
@@ -2090,68 +2188,71 @@
         <v>2</v>
       </c>
       <c r="D29" s="1">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
       <c r="F29" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>21</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
         <v>13</v>
-      </c>
-      <c r="H29" s="1">
-        <v>0</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0</v>
-      </c>
-      <c r="J29" s="1">
-        <v>0</v>
-      </c>
-      <c r="K29" s="1">
-        <v>0</v>
-      </c>
-      <c r="L29" s="1">
-        <v>0</v>
-      </c>
-      <c r="M29" s="1">
-        <v>0</v>
-      </c>
-      <c r="N29" s="1">
-        <v>0</v>
-      </c>
-      <c r="O29" s="1">
-        <v>0</v>
-      </c>
-      <c r="P29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C30" s="1">
-        <v>2</v>
-      </c>
-      <c r="D30" s="1">
-        <v>22</v>
-      </c>
-      <c r="E30" s="1">
-        <v>2</v>
-      </c>
-      <c r="F30" s="1">
-        <v>3</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H30" s="1">
         <v>0</v>
@@ -2180,10 +2281,13 @@
       <c r="P30" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B31" s="1">
         <v>2025</v>
@@ -2195,14 +2299,14 @@
         <v>22</v>
       </c>
       <c r="E31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H31" s="1">
         <v>0</v>
@@ -2231,29 +2335,32 @@
       <c r="P31" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
         <v>22</v>
       </c>
-      <c r="B32" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C32" s="1">
-        <v>2</v>
-      </c>
-      <c r="D32" s="1">
-        <v>24</v>
-      </c>
       <c r="E32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="1">
         <v>0</v>
@@ -2265,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L32" s="1">
         <v>0</v>
@@ -2282,10 +2389,13 @@
       <c r="P32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B33" s="1">
         <v>2025</v>
@@ -2313,81 +2423,87 @@
         <v>0</v>
       </c>
       <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>9</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>24</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1">
         <v>6</v>
       </c>
-      <c r="K33" s="1">
-        <v>0</v>
-      </c>
-      <c r="L33" s="1">
-        <v>0</v>
-      </c>
-      <c r="M33" s="1">
-        <v>0</v>
-      </c>
-      <c r="N33" s="1">
-        <v>0</v>
-      </c>
-      <c r="O33" s="1">
-        <v>0</v>
-      </c>
-      <c r="P33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0</v>
+      </c>
+      <c r="P34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B34" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C34" s="1">
-        <v>2</v>
-      </c>
-      <c r="D34" s="1">
-        <v>25</v>
-      </c>
-      <c r="E34" s="1">
-        <v>0</v>
-      </c>
-      <c r="F34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" s="1">
-        <f t="shared" ref="G34:G86" si="1">SUM(E34:F34)</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="1">
-        <v>0</v>
-      </c>
-      <c r="I34" s="1">
-        <v>0</v>
-      </c>
-      <c r="J34" s="1">
-        <v>11</v>
-      </c>
-      <c r="K34" s="1">
-        <v>0</v>
-      </c>
-      <c r="L34" s="1">
-        <v>0</v>
-      </c>
-      <c r="M34" s="1">
-        <v>0</v>
-      </c>
-      <c r="N34" s="1">
-        <v>0</v>
-      </c>
-      <c r="O34" s="1">
-        <v>0</v>
-      </c>
-      <c r="P34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>2025</v>
@@ -2399,14 +2515,14 @@
         <v>25</v>
       </c>
       <c r="E35" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" ref="G35:G72" si="1">SUM(E35:F35)</f>
+        <v>0</v>
       </c>
       <c r="H35" s="1">
         <v>0</v>
@@ -2415,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K35" s="1">
         <v>0</v>
@@ -2435,10 +2551,13 @@
       <c r="P35" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1">
         <v>2025</v>
@@ -2450,14 +2569,14 @@
         <v>25</v>
       </c>
       <c r="E36" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
       </c>
       <c r="G36" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" s="1">
         <v>0</v>
@@ -2469,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="L36" s="1">
         <v>0</v>
@@ -2486,10 +2605,13 @@
       <c r="P36" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B37" s="1">
         <v>2025</v>
@@ -2498,17 +2620,17 @@
         <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" s="1">
         <v>0</v>
@@ -2520,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L37" s="1">
         <v>0</v>
@@ -2537,29 +2659,32 @@
       <c r="P37" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B38" s="1">
         <v>2025</v>
       </c>
       <c r="C38" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
       </c>
       <c r="G38" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="1">
         <v>0</v>
@@ -2571,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L38" s="1">
         <v>0</v>
@@ -2588,10 +2713,13 @@
       <c r="P38" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B39" s="1">
         <v>2025</v>
@@ -2603,14 +2731,14 @@
         <v>1</v>
       </c>
       <c r="E39" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H39" s="1">
         <v>0</v>
@@ -2619,10 +2747,10 @@
         <v>0</v>
       </c>
       <c r="J39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L39" s="1">
         <v>0</v>
@@ -2639,10 +2767,13 @@
       <c r="P39" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1">
         <v>2025</v>
@@ -2654,14 +2785,14 @@
         <v>1</v>
       </c>
       <c r="E40" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
       </c>
       <c r="G40" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H40" s="1">
         <v>0</v>
@@ -2670,10 +2801,10 @@
         <v>0</v>
       </c>
       <c r="J40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L40" s="1">
         <v>0</v>
@@ -2690,10 +2821,13 @@
       <c r="P40" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1">
         <v>2025</v>
@@ -2702,7 +2836,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -2721,10 +2855,10 @@
         <v>0</v>
       </c>
       <c r="J41" s="1">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="K41" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L41" s="1">
         <v>0</v>
@@ -2741,10 +2875,13 @@
       <c r="P41" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1">
         <v>2025</v>
@@ -2772,10 +2909,10 @@
         <v>0</v>
       </c>
       <c r="J42" s="1">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="K42" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="L42" s="1">
         <v>0</v>
@@ -2792,10 +2929,13 @@
       <c r="P42" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1">
         <v>2025</v>
@@ -2823,10 +2963,10 @@
         <v>0</v>
       </c>
       <c r="J43" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K43" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="L43" s="1">
         <v>0</v>
@@ -2843,10 +2983,13 @@
       <c r="P43" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B44" s="1">
         <v>2025</v>
@@ -2874,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="1">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="K44" s="1">
         <v>0</v>
@@ -2894,10 +3037,13 @@
       <c r="P44" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1">
         <v>2025</v>
@@ -2906,7 +3052,7 @@
         <v>3</v>
       </c>
       <c r="D45" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -2925,10 +3071,10 @@
         <v>0</v>
       </c>
       <c r="J45" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K45" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L45" s="1">
         <v>0</v>
@@ -2945,10 +3091,13 @@
       <c r="P45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B46" s="1">
         <v>2025</v>
@@ -2960,14 +3109,14 @@
         <v>3</v>
       </c>
       <c r="E46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H46" s="1">
         <v>0</v>
@@ -2979,7 +3128,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L46" s="1">
         <v>0</v>
@@ -2996,10 +3145,13 @@
       <c r="P46" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B47" s="1">
         <v>2025</v>
@@ -3011,14 +3163,14 @@
         <v>3</v>
       </c>
       <c r="E47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H47" s="1">
         <v>0</v>
@@ -3039,7 +3191,7 @@
         <v>0</v>
       </c>
       <c r="N47" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O47" s="1">
         <v>0</v>
@@ -3047,10 +3199,13 @@
       <c r="P47" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="1">
         <v>2025</v>
@@ -3098,10 +3253,13 @@
       <c r="P48" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1">
         <v>2025</v>
@@ -3113,14 +3271,14 @@
         <v>3</v>
       </c>
       <c r="E49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" s="1">
         <v>0</v>
@@ -3141,18 +3299,21 @@
         <v>0</v>
       </c>
       <c r="N49" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P49" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1">
         <v>2025</v>
@@ -3161,17 +3322,17 @@
         <v>3</v>
       </c>
       <c r="D50" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H50" s="1">
         <v>0</v>
@@ -3195,15 +3356,18 @@
         <v>0</v>
       </c>
       <c r="O50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" s="1">
         <v>2025</v>
@@ -3212,13 +3376,13 @@
         <v>3</v>
       </c>
       <c r="D51" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E51" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" si="1"/>
@@ -3234,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="K51" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L51" s="1">
         <v>0</v>
@@ -3251,10 +3415,13 @@
       <c r="P51" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B52" s="1">
         <v>2025</v>
@@ -3266,14 +3433,14 @@
         <v>5</v>
       </c>
       <c r="E52" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
       </c>
       <c r="G52" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H52" s="1">
         <v>0</v>
@@ -3285,7 +3452,7 @@
         <v>0</v>
       </c>
       <c r="K52" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L52" s="1">
         <v>0</v>
@@ -3302,10 +3469,13 @@
       <c r="P52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B53" s="1">
         <v>2025</v>
@@ -3314,13 +3484,13 @@
         <v>3</v>
       </c>
       <c r="D53" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53" s="1">
         <f t="shared" si="1"/>
@@ -3330,7 +3500,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" s="1">
         <v>0</v>
@@ -3353,10 +3523,13 @@
       <c r="P53" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1">
         <v>2025</v>
@@ -3371,20 +3544,20 @@
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54" s="1">
         <v>0</v>
       </c>
       <c r="I54" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K54" s="1">
         <v>0</v>
@@ -3404,10 +3577,13 @@
       <c r="P54" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" s="1">
         <v>2025</v>
@@ -3435,10 +3611,10 @@
         <v>0</v>
       </c>
       <c r="J55" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K55" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="L55" s="1">
         <v>0</v>
@@ -3455,10 +3631,13 @@
       <c r="P55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B56" s="1">
         <v>2025</v>
@@ -3489,7 +3668,7 @@
         <v>0</v>
       </c>
       <c r="K56" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L56" s="1">
         <v>0</v>
@@ -3504,12 +3683,15 @@
         <v>0</v>
       </c>
       <c r="P56" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B57" s="1">
         <v>2025</v>
@@ -3518,17 +3700,17 @@
         <v>3</v>
       </c>
       <c r="D57" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H57" s="1">
         <v>0</v>
@@ -3555,12 +3737,15 @@
         <v>0</v>
       </c>
       <c r="P57" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1">
         <v>2025</v>
@@ -3572,14 +3757,14 @@
         <v>7</v>
       </c>
       <c r="E58" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H58" s="1">
         <v>0</v>
@@ -3591,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="K58" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L58" s="1">
         <v>0</v>
@@ -3608,10 +3793,13 @@
       <c r="P58" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1">
         <v>2025</v>
@@ -3642,7 +3830,7 @@
         <v>0</v>
       </c>
       <c r="K59" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L59" s="1">
         <v>0</v>
@@ -3659,10 +3847,13 @@
       <c r="P59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B60" s="1">
         <v>2025</v>
@@ -3671,7 +3862,7 @@
         <v>3</v>
       </c>
       <c r="D60" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
@@ -3690,10 +3881,10 @@
         <v>0</v>
       </c>
       <c r="J60" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K60" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L60" s="1">
         <v>0</v>
@@ -3702,7 +3893,7 @@
         <v>0</v>
       </c>
       <c r="N60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O60" s="1">
         <v>0</v>
@@ -3710,10 +3901,13 @@
       <c r="P60" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" s="1">
         <v>2025</v>
@@ -3722,7 +3916,7 @@
         <v>3</v>
       </c>
       <c r="D61" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>
@@ -3741,10 +3935,10 @@
         <v>0</v>
       </c>
       <c r="J61" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K61" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L61" s="1">
         <v>0</v>
@@ -3753,7 +3947,7 @@
         <v>0</v>
       </c>
       <c r="N61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O61" s="1">
         <v>0</v>
@@ -3761,10 +3955,13 @@
       <c r="P61" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1">
         <v>2025</v>
@@ -3792,10 +3989,10 @@
         <v>0</v>
       </c>
       <c r="J62" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K62" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L62" s="1">
         <v>0</v>
@@ -3812,10 +4009,13 @@
       <c r="P62" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1">
         <v>2025</v>
@@ -3824,7 +4024,7 @@
         <v>3</v>
       </c>
       <c r="D63" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E63" s="1">
         <v>0</v>
@@ -3843,7 +4043,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K63" s="1">
         <v>0</v>
@@ -3863,10 +4063,13 @@
       <c r="P63" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B64" s="1">
         <v>2025</v>
@@ -3875,17 +4078,17 @@
         <v>3</v>
       </c>
       <c r="D64" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E64" s="1">
         <v>0</v>
       </c>
       <c r="F64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" s="1">
         <v>0</v>
@@ -3894,7 +4097,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="K64" s="1">
         <v>0</v>
@@ -3912,12 +4115,15 @@
         <v>0</v>
       </c>
       <c r="P64" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="1">
         <v>2025</v>
@@ -3926,17 +4132,17 @@
         <v>3</v>
       </c>
       <c r="D65" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E65" s="1">
         <v>0</v>
       </c>
       <c r="F65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="1">
         <v>0</v>
@@ -3945,7 +4151,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="1">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="K65" s="1">
         <v>0</v>
@@ -3963,12 +4169,15 @@
         <v>0</v>
       </c>
       <c r="P65" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="1">
         <v>2025</v>
@@ -3996,7 +4205,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="1">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="K66" s="1">
         <v>0</v>
@@ -4016,11 +4225,13 @@
       <c r="P66" s="1">
         <v>0</v>
       </c>
-      <c r="Q66" s="1"/>
+      <c r="Q66" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B67" s="1">
         <v>2025</v>
@@ -4048,7 +4259,7 @@
         <v>0</v>
       </c>
       <c r="J67" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K67" s="1">
         <v>0</v>
@@ -4066,12 +4277,15 @@
         <v>0</v>
       </c>
       <c r="P67" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B68" s="1">
         <v>2025</v>
@@ -4080,17 +4294,17 @@
         <v>3</v>
       </c>
       <c r="D68" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E68" s="1">
         <v>0</v>
       </c>
       <c r="F68" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G68" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H68" s="1">
         <v>0</v>
@@ -4099,10 +4313,10 @@
         <v>0</v>
       </c>
       <c r="J68" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K68" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L68" s="1">
         <v>0</v>
@@ -4119,11 +4333,13 @@
       <c r="P68" s="1">
         <v>0</v>
       </c>
-      <c r="Q68" s="1"/>
+      <c r="Q68" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B69" s="1">
         <v>2025</v>
@@ -4138,11 +4354,11 @@
         <v>0</v>
       </c>
       <c r="F69" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G69" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H69" s="1">
         <v>0</v>
@@ -4151,10 +4367,10 @@
         <v>0</v>
       </c>
       <c r="J69" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K69" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L69" s="1">
         <v>0</v>
@@ -4169,12 +4385,15 @@
         <v>0</v>
       </c>
       <c r="P69" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B70" s="1">
         <v>2025</v>
@@ -4183,7 +4402,7 @@
         <v>3</v>
       </c>
       <c r="D70" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E70" s="1">
         <v>0</v>
@@ -4202,30 +4421,249 @@
         <v>0</v>
       </c>
       <c r="J70" s="1">
+        <v>17</v>
+      </c>
+      <c r="K70" s="1">
+        <v>0</v>
+      </c>
+      <c r="L70" s="1">
+        <v>0</v>
+      </c>
+      <c r="M70" s="1">
+        <v>0</v>
+      </c>
+      <c r="N70" s="1">
+        <v>0</v>
+      </c>
+      <c r="O70" s="1">
+        <v>0</v>
+      </c>
+      <c r="P70" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C71" s="1">
+        <v>3</v>
+      </c>
+      <c r="D71" s="1">
+        <v>19</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H71" s="1">
+        <v>0</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0</v>
+      </c>
+      <c r="J71" s="1">
         <v>7</v>
       </c>
-      <c r="K70" s="1">
-        <v>0</v>
-      </c>
-      <c r="L70" s="1">
-        <v>0</v>
-      </c>
-      <c r="M70" s="1">
-        <v>0</v>
-      </c>
-      <c r="N70" s="1">
-        <v>0</v>
-      </c>
-      <c r="O70" s="1">
-        <v>0</v>
-      </c>
-      <c r="P70" s="1">
+      <c r="K71" s="1">
+        <v>0</v>
+      </c>
+      <c r="L71" s="1">
+        <v>0</v>
+      </c>
+      <c r="M71" s="1">
+        <v>0</v>
+      </c>
+      <c r="N71" s="1">
+        <v>0</v>
+      </c>
+      <c r="O71" s="1">
+        <v>0</v>
+      </c>
+      <c r="P71" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C72" s="1">
+        <v>3</v>
+      </c>
+      <c r="D72" s="1">
+        <v>24</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0</v>
+      </c>
+      <c r="J72" s="1">
+        <v>0</v>
+      </c>
+      <c r="K72" s="1">
+        <v>1</v>
+      </c>
+      <c r="L72" s="1">
+        <v>0</v>
+      </c>
+      <c r="M72" s="1">
+        <v>0</v>
+      </c>
+      <c r="N72" s="1">
+        <v>0</v>
+      </c>
+      <c r="O72" s="1">
+        <v>0</v>
+      </c>
+      <c r="P72" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B73" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C73" s="1">
+        <v>3</v>
+      </c>
+      <c r="D73" s="1">
+        <v>24</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0</v>
+      </c>
+      <c r="F73" s="1">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1">
+        <f t="shared" ref="G73:G74" si="2">SUM(E73:F73)</f>
+        <v>0</v>
+      </c>
+      <c r="H73" s="1">
+        <v>0</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0</v>
+      </c>
+      <c r="J73" s="1">
+        <v>0</v>
+      </c>
+      <c r="K73" s="1">
+        <v>1</v>
+      </c>
+      <c r="L73" s="1">
+        <v>0</v>
+      </c>
+      <c r="M73" s="1">
+        <v>0</v>
+      </c>
+      <c r="N73" s="1">
+        <v>0</v>
+      </c>
+      <c r="O73" s="1">
+        <v>0</v>
+      </c>
+      <c r="P73" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C74" s="1">
+        <v>3</v>
+      </c>
+      <c r="D74" s="1">
+        <v>24</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0</v>
+      </c>
+      <c r="F74" s="1">
+        <v>0</v>
+      </c>
+      <c r="G74" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H74" s="1">
+        <v>0</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0</v>
+      </c>
+      <c r="J74" s="1">
+        <v>0</v>
+      </c>
+      <c r="K74" s="1">
+        <v>1</v>
+      </c>
+      <c r="L74" s="1">
+        <v>0</v>
+      </c>
+      <c r="M74" s="1">
+        <v>0</v>
+      </c>
+      <c r="N74" s="1">
+        <v>0</v>
+      </c>
+      <c r="O74" s="1">
+        <v>0</v>
+      </c>
+      <c r="P74" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P63">
-    <sortCondition ref="A2:A63"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P64">
+    <sortCondition ref="A2:A64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: adding data from trail cams
</commit_message>
<xml_diff>
--- a/data/Truth.xlsx
+++ b/data/Truth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\AI Projects\otter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CD0674-50C0-41AD-860B-76247B330444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65867C53-7CA8-4C68-9FB5-BA062A07FA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30450" yWindow="2745" windowWidth="24330" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Image</t>
   </si>
@@ -337,6 +337,27 @@
   </si>
   <si>
     <t>250401_MLTRE_0</t>
+  </si>
+  <si>
+    <t>250411_KEN1_0</t>
+  </si>
+  <si>
+    <t>250410_KEN1_0</t>
+  </si>
+  <si>
+    <t>250410_BSHNL_0</t>
+  </si>
+  <si>
+    <t>250411_BSHNL_0</t>
+  </si>
+  <si>
+    <t>250413_BSHNL_0</t>
+  </si>
+  <si>
+    <t>250414_BSHNL_0</t>
+  </si>
+  <si>
+    <t>250415_KEN1_0</t>
   </si>
 </sst>
 </file>
@@ -684,7 +705,7 @@
   <dimension ref="A1:Q921"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q88" sqref="Q88"/>
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4810,7 +4831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>85</v>
       </c>
@@ -4864,7 +4885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>86</v>
       </c>
@@ -4918,7 +4939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>87</v>
       </c>
@@ -4972,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>95</v>
       </c>
@@ -5026,7 +5047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>96</v>
       </c>
@@ -5046,7 +5067,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="1">
-        <f t="shared" ref="G81:G88" si="5">SUM(E81:F81)</f>
+        <f t="shared" ref="G81:G95" si="5">SUM(E81:F81)</f>
         <v>0</v>
       </c>
       <c r="H81" s="1">
@@ -5080,7 +5101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>97</v>
       </c>
@@ -5134,7 +5155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>98</v>
       </c>
@@ -5188,7 +5209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>99</v>
       </c>
@@ -5242,7 +5263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>100</v>
       </c>
@@ -5296,7 +5317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>101</v>
       </c>
@@ -5350,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>102</v>
       </c>
@@ -5459,53 +5480,382 @@
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M89" s="1"/>
-      <c r="N89" s="1"/>
-      <c r="O89" s="1"/>
-      <c r="P89" s="1"/>
-      <c r="Q89" s="1"/>
+      <c r="A89" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B89" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C89" s="1">
+        <v>4</v>
+      </c>
+      <c r="D89" s="1">
+        <v>10</v>
+      </c>
+      <c r="E89" s="1">
+        <v>0</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0</v>
+      </c>
+      <c r="I89" s="1">
+        <v>0</v>
+      </c>
+      <c r="J89" s="1">
+        <v>2</v>
+      </c>
+      <c r="K89" s="1">
+        <v>0</v>
+      </c>
+      <c r="L89" s="1">
+        <v>0</v>
+      </c>
+      <c r="M89" s="1">
+        <v>0</v>
+      </c>
+      <c r="N89" s="1">
+        <v>0</v>
+      </c>
+      <c r="O89" s="1">
+        <v>0</v>
+      </c>
+      <c r="P89" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q89" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M90" s="1"/>
-      <c r="N90" s="1"/>
-      <c r="O90" s="1"/>
-      <c r="P90" s="1"/>
-      <c r="Q90" s="1"/>
+      <c r="A90" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B90" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C90" s="1">
+        <v>4</v>
+      </c>
+      <c r="D90" s="1">
+        <v>10</v>
+      </c>
+      <c r="E90" s="1">
+        <v>0</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H90" s="1">
+        <v>0</v>
+      </c>
+      <c r="I90" s="1">
+        <v>0</v>
+      </c>
+      <c r="J90" s="1">
+        <v>0</v>
+      </c>
+      <c r="K90" s="1">
+        <v>15</v>
+      </c>
+      <c r="L90" s="1">
+        <v>0</v>
+      </c>
+      <c r="M90" s="1">
+        <v>0</v>
+      </c>
+      <c r="N90" s="1">
+        <v>0</v>
+      </c>
+      <c r="O90" s="1">
+        <v>0</v>
+      </c>
+      <c r="P90" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q90" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M91" s="1"/>
-      <c r="N91" s="1"/>
-      <c r="O91" s="1"/>
-      <c r="P91" s="1"/>
-      <c r="Q91" s="1"/>
+      <c r="A91" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B91" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C91" s="1">
+        <v>4</v>
+      </c>
+      <c r="D91" s="1">
+        <v>11</v>
+      </c>
+      <c r="E91" s="1">
+        <v>0</v>
+      </c>
+      <c r="F91" s="1">
+        <v>0</v>
+      </c>
+      <c r="G91" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H91" s="1">
+        <v>0</v>
+      </c>
+      <c r="I91" s="1">
+        <v>0</v>
+      </c>
+      <c r="J91" s="1">
+        <v>1</v>
+      </c>
+      <c r="K91" s="1">
+        <v>0</v>
+      </c>
+      <c r="L91" s="1">
+        <v>0</v>
+      </c>
+      <c r="M91" s="1">
+        <v>0</v>
+      </c>
+      <c r="N91" s="1">
+        <v>0</v>
+      </c>
+      <c r="O91" s="1">
+        <v>0</v>
+      </c>
+      <c r="P91" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q91" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M92" s="1"/>
-      <c r="N92" s="1"/>
-      <c r="O92" s="1"/>
-      <c r="P92" s="1"/>
-      <c r="Q92" s="1"/>
+      <c r="A92" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B92" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C92" s="1">
+        <v>4</v>
+      </c>
+      <c r="D92" s="1">
+        <v>11</v>
+      </c>
+      <c r="E92" s="1">
+        <v>0</v>
+      </c>
+      <c r="F92" s="1">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H92" s="1">
+        <v>0</v>
+      </c>
+      <c r="I92" s="1">
+        <v>0</v>
+      </c>
+      <c r="J92" s="1">
+        <v>1</v>
+      </c>
+      <c r="K92" s="1">
+        <v>0</v>
+      </c>
+      <c r="L92" s="1">
+        <v>0</v>
+      </c>
+      <c r="M92" s="1">
+        <v>0</v>
+      </c>
+      <c r="N92" s="1">
+        <v>0</v>
+      </c>
+      <c r="O92" s="1">
+        <v>0</v>
+      </c>
+      <c r="P92" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M93" s="1"/>
-      <c r="N93" s="1"/>
-      <c r="O93" s="1"/>
-      <c r="P93" s="1"/>
-      <c r="Q93" s="1"/>
+      <c r="A93" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B93" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C93" s="1">
+        <v>4</v>
+      </c>
+      <c r="D93" s="1">
+        <v>13</v>
+      </c>
+      <c r="E93" s="1">
+        <v>0</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0</v>
+      </c>
+      <c r="G93" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H93" s="1">
+        <v>0</v>
+      </c>
+      <c r="I93" s="1">
+        <v>0</v>
+      </c>
+      <c r="J93" s="1">
+        <v>2</v>
+      </c>
+      <c r="K93" s="1">
+        <v>0</v>
+      </c>
+      <c r="L93" s="1">
+        <v>0</v>
+      </c>
+      <c r="M93" s="1">
+        <v>0</v>
+      </c>
+      <c r="N93" s="1">
+        <v>0</v>
+      </c>
+      <c r="O93" s="1">
+        <v>0</v>
+      </c>
+      <c r="P93" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M94" s="1"/>
-      <c r="N94" s="1"/>
-      <c r="O94" s="1"/>
-      <c r="P94" s="1"/>
-      <c r="Q94" s="1"/>
+      <c r="A94" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B94" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C94" s="1">
+        <v>4</v>
+      </c>
+      <c r="D94" s="1">
+        <v>14</v>
+      </c>
+      <c r="E94" s="1">
+        <v>0</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0</v>
+      </c>
+      <c r="G94" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H94" s="1">
+        <v>0</v>
+      </c>
+      <c r="I94" s="1">
+        <v>0</v>
+      </c>
+      <c r="J94" s="1">
+        <v>5</v>
+      </c>
+      <c r="K94" s="1">
+        <v>0</v>
+      </c>
+      <c r="L94" s="1">
+        <v>0</v>
+      </c>
+      <c r="M94" s="1">
+        <v>0</v>
+      </c>
+      <c r="N94" s="1">
+        <v>0</v>
+      </c>
+      <c r="O94" s="1">
+        <v>0</v>
+      </c>
+      <c r="P94" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M95" s="1"/>
-      <c r="N95" s="1"/>
-      <c r="O95" s="1"/>
-      <c r="P95" s="1"/>
-      <c r="Q95" s="1"/>
+      <c r="A95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B95" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C95" s="1">
+        <v>4</v>
+      </c>
+      <c r="D95" s="1">
+        <v>15</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1">
+        <v>0</v>
+      </c>
+      <c r="G95" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H95" s="1">
+        <v>0</v>
+      </c>
+      <c r="I95" s="1">
+        <v>0</v>
+      </c>
+      <c r="J95" s="1">
+        <v>4</v>
+      </c>
+      <c r="K95" s="1">
+        <v>0</v>
+      </c>
+      <c r="L95" s="1">
+        <v>0</v>
+      </c>
+      <c r="M95" s="1">
+        <v>0</v>
+      </c>
+      <c r="N95" s="1">
+        <v>0</v>
+      </c>
+      <c r="O95" s="1">
+        <v>0</v>
+      </c>
+      <c r="P95" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M96" s="1"/>

</xml_diff>

<commit_message>
chore: regular data add
</commit_message>
<xml_diff>
--- a/data/Truth.xlsx
+++ b/data/Truth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\AI Projects\otter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBC1B99-2994-4B37-8D1F-7C73C0F9E613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24552679-F3F1-472F-8465-3F5C1DB34C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31740" yWindow="1740" windowWidth="19275" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="5445" windowWidth="19275" windowHeight="9630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Image</t>
   </si>
@@ -367,6 +367,24 @@
   </si>
   <si>
     <t>250421_TRLCAM_0</t>
+  </si>
+  <si>
+    <t>250422_KEN1_0</t>
+  </si>
+  <si>
+    <t>250424_KEN1_0</t>
+  </si>
+  <si>
+    <t>250425_KEN1_0</t>
+  </si>
+  <si>
+    <t>250426_STLTH_0</t>
+  </si>
+  <si>
+    <t>250427_KEN1_0</t>
+  </si>
+  <si>
+    <t>250427_KEN1_1</t>
   </si>
 </sst>
 </file>
@@ -714,7 +732,7 @@
   <dimension ref="A1:Q921"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R98" sqref="R98"/>
+      <selection activeCell="M101" sqref="M101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5076,7 +5094,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="1">
-        <f t="shared" ref="G81:G98" si="5">SUM(E81:F81)</f>
+        <f t="shared" ref="G81:G104" si="5">SUM(E81:F81)</f>
         <v>0</v>
       </c>
       <c r="H81" s="1">
@@ -5434,7 +5452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>103</v>
       </c>
@@ -5488,7 +5506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>106</v>
       </c>
@@ -5542,7 +5560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>105</v>
       </c>
@@ -5596,7 +5614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>107</v>
       </c>
@@ -5650,7 +5668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>104</v>
       </c>
@@ -5704,7 +5722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>108</v>
       </c>
@@ -5758,7 +5776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>109</v>
       </c>
@@ -5812,7 +5830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>110</v>
       </c>
@@ -5866,7 +5884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>111</v>
       </c>
@@ -5920,7 +5938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>112</v>
       </c>
@@ -5974,7 +5992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>113</v>
       </c>
@@ -6029,46 +6047,328 @@
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M99" s="1"/>
-      <c r="N99" s="1"/>
-      <c r="O99" s="1"/>
-      <c r="P99" s="1"/>
-      <c r="Q99" s="1"/>
+      <c r="A99" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B99" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C99" s="1">
+        <v>4</v>
+      </c>
+      <c r="D99" s="1">
+        <v>22</v>
+      </c>
+      <c r="E99" s="1">
+        <v>2</v>
+      </c>
+      <c r="F99" s="1">
+        <v>0</v>
+      </c>
+      <c r="G99" s="1">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H99" s="1">
+        <v>0</v>
+      </c>
+      <c r="I99" s="1">
+        <v>0</v>
+      </c>
+      <c r="J99" s="1">
+        <v>4</v>
+      </c>
+      <c r="K99" s="1">
+        <v>1</v>
+      </c>
+      <c r="L99" s="1">
+        <v>0</v>
+      </c>
+      <c r="M99" s="1">
+        <v>0</v>
+      </c>
+      <c r="N99" s="1">
+        <v>0</v>
+      </c>
+      <c r="O99" s="1">
+        <v>0</v>
+      </c>
+      <c r="P99" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
-      <c r="O100" s="1"/>
-      <c r="P100" s="1"/>
-      <c r="Q100" s="1"/>
+      <c r="A100" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B100" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C100" s="1">
+        <v>4</v>
+      </c>
+      <c r="D100" s="1">
+        <v>24</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0</v>
+      </c>
+      <c r="F100" s="1">
+        <v>0</v>
+      </c>
+      <c r="G100" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H100" s="1">
+        <v>0</v>
+      </c>
+      <c r="I100" s="1">
+        <v>0</v>
+      </c>
+      <c r="J100" s="1">
+        <v>5</v>
+      </c>
+      <c r="K100" s="1">
+        <v>0</v>
+      </c>
+      <c r="L100" s="1">
+        <v>0</v>
+      </c>
+      <c r="M100" s="1">
+        <v>0</v>
+      </c>
+      <c r="N100" s="1">
+        <v>0</v>
+      </c>
+      <c r="O100" s="1">
+        <v>0</v>
+      </c>
+      <c r="P100" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q100" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
-      <c r="O101" s="1"/>
-      <c r="P101" s="1"/>
-      <c r="Q101" s="1"/>
+      <c r="A101" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B101" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C101" s="1">
+        <v>4</v>
+      </c>
+      <c r="D101" s="1">
+        <v>25</v>
+      </c>
+      <c r="E101" s="1">
+        <v>2</v>
+      </c>
+      <c r="F101" s="1">
+        <v>1</v>
+      </c>
+      <c r="G101" s="1">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="H101" s="1">
+        <v>0</v>
+      </c>
+      <c r="I101" s="1">
+        <v>0</v>
+      </c>
+      <c r="J101" s="1">
+        <v>0</v>
+      </c>
+      <c r="K101" s="1">
+        <v>0</v>
+      </c>
+      <c r="L101" s="1">
+        <v>0</v>
+      </c>
+      <c r="M101" s="1">
+        <v>0</v>
+      </c>
+      <c r="N101" s="1">
+        <v>0</v>
+      </c>
+      <c r="O101" s="1">
+        <v>0</v>
+      </c>
+      <c r="P101" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q101" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
-      <c r="O102" s="1"/>
-      <c r="P102" s="1"/>
-      <c r="Q102" s="1"/>
+      <c r="A102" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B102" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C102" s="1">
+        <v>4</v>
+      </c>
+      <c r="D102" s="1">
+        <v>26</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1</v>
+      </c>
+      <c r="F102" s="1">
+        <v>0</v>
+      </c>
+      <c r="G102" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H102" s="1">
+        <v>0</v>
+      </c>
+      <c r="I102" s="1">
+        <v>0</v>
+      </c>
+      <c r="J102" s="1">
+        <v>0</v>
+      </c>
+      <c r="K102" s="1">
+        <v>0</v>
+      </c>
+      <c r="L102" s="1">
+        <v>0</v>
+      </c>
+      <c r="M102" s="1">
+        <v>0</v>
+      </c>
+      <c r="N102" s="1">
+        <v>0</v>
+      </c>
+      <c r="O102" s="1">
+        <v>0</v>
+      </c>
+      <c r="P102" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q102" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
-      <c r="O103" s="1"/>
-      <c r="P103" s="1"/>
-      <c r="Q103" s="1"/>
+      <c r="A103" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B103" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C103" s="1">
+        <v>4</v>
+      </c>
+      <c r="D103" s="1">
+        <v>27</v>
+      </c>
+      <c r="E103" s="1">
+        <v>1</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0</v>
+      </c>
+      <c r="G103" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H103" s="1">
+        <v>0</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0</v>
+      </c>
+      <c r="J103" s="1">
+        <v>0</v>
+      </c>
+      <c r="K103" s="1">
+        <v>2</v>
+      </c>
+      <c r="L103" s="1">
+        <v>0</v>
+      </c>
+      <c r="M103" s="1">
+        <v>0</v>
+      </c>
+      <c r="N103" s="1">
+        <v>0</v>
+      </c>
+      <c r="O103" s="1">
+        <v>0</v>
+      </c>
+      <c r="P103" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
-      <c r="O104" s="1"/>
-      <c r="P104" s="1"/>
-      <c r="Q104" s="1"/>
+      <c r="A104" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B104" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C104" s="1">
+        <v>4</v>
+      </c>
+      <c r="D104" s="1">
+        <v>27</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0</v>
+      </c>
+      <c r="G104" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H104" s="1">
+        <v>0</v>
+      </c>
+      <c r="I104" s="1">
+        <v>0</v>
+      </c>
+      <c r="J104" s="1">
+        <v>0</v>
+      </c>
+      <c r="K104" s="1">
+        <v>2</v>
+      </c>
+      <c r="L104" s="1">
+        <v>0</v>
+      </c>
+      <c r="M104" s="1">
+        <v>0</v>
+      </c>
+      <c r="N104" s="1">
+        <v>0</v>
+      </c>
+      <c r="O104" s="1">
+        <v>0</v>
+      </c>
+      <c r="P104" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q104" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M105" s="1"/>

</xml_diff>

<commit_message>
chore: adding more data
</commit_message>
<xml_diff>
--- a/data/Truth.xlsx
+++ b/data/Truth.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\AI Projects\otter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CD82F7-03A0-4532-97EF-861517043FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A50D79D4-0FD2-4904-BE4A-349EFC23B56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="3555" windowWidth="17595" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>Image</t>
   </si>
@@ -400,6 +411,21 @@
   </si>
   <si>
     <t>250504_STLTH_0</t>
+  </si>
+  <si>
+    <t>250526_BSHNL_0</t>
+  </si>
+  <si>
+    <t>250525_STLTH_0</t>
+  </si>
+  <si>
+    <t>250523_BSHNL_0</t>
+  </si>
+  <si>
+    <t>250528_STLTH_0</t>
+  </si>
+  <si>
+    <t>250608_TC1_0</t>
   </si>
 </sst>
 </file>
@@ -744,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q921"/>
+  <dimension ref="A1:R921"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q107" sqref="Q107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5109,7 +5135,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="1">
-        <f t="shared" ref="G81:G109" si="5">SUM(E81:F81)</f>
+        <f t="shared" ref="G81:G114" si="5">SUM(E81:F81)</f>
         <v>0</v>
       </c>
       <c r="H81" s="1">
@@ -6656,132 +6682,368 @@
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M110" s="1"/>
-      <c r="N110" s="1"/>
-      <c r="O110" s="1"/>
-      <c r="P110" s="1"/>
-      <c r="Q110" s="1"/>
+      <c r="A110" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B110" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C110" s="1">
+        <v>5</v>
+      </c>
+      <c r="D110" s="1">
+        <v>23</v>
+      </c>
+      <c r="E110" s="1">
+        <v>0</v>
+      </c>
+      <c r="F110" s="1">
+        <v>1</v>
+      </c>
+      <c r="G110" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0</v>
+      </c>
+      <c r="I110" s="1">
+        <v>0</v>
+      </c>
+      <c r="J110" s="1">
+        <v>0</v>
+      </c>
+      <c r="K110" s="1">
+        <v>0</v>
+      </c>
+      <c r="L110" s="1">
+        <v>0</v>
+      </c>
+      <c r="M110" s="1">
+        <v>0</v>
+      </c>
+      <c r="N110" s="1">
+        <v>0</v>
+      </c>
+      <c r="O110" s="1">
+        <v>0</v>
+      </c>
+      <c r="P110" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q110" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M111" s="1"/>
-      <c r="N111" s="1"/>
-      <c r="O111" s="1"/>
-      <c r="P111" s="1"/>
-      <c r="Q111" s="1"/>
+      <c r="A111" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B111" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C111" s="1">
+        <v>5</v>
+      </c>
+      <c r="D111" s="1">
+        <v>25</v>
+      </c>
+      <c r="E111" s="1">
+        <v>1</v>
+      </c>
+      <c r="F111" s="1">
+        <v>0</v>
+      </c>
+      <c r="G111" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H111" s="1">
+        <v>0</v>
+      </c>
+      <c r="I111" s="1">
+        <v>0</v>
+      </c>
+      <c r="J111" s="1">
+        <v>0</v>
+      </c>
+      <c r="K111" s="1">
+        <v>0</v>
+      </c>
+      <c r="L111" s="1">
+        <v>0</v>
+      </c>
+      <c r="M111" s="1">
+        <v>0</v>
+      </c>
+      <c r="N111" s="1">
+        <v>0</v>
+      </c>
+      <c r="O111" s="1">
+        <v>0</v>
+      </c>
+      <c r="P111" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q111" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M112" s="1"/>
-      <c r="N112" s="1"/>
-      <c r="O112" s="1"/>
-      <c r="P112" s="1"/>
-      <c r="Q112" s="1"/>
-    </row>
-    <row r="113" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M113" s="1"/>
-      <c r="N113" s="1"/>
-      <c r="O113" s="1"/>
-      <c r="P113" s="1"/>
-      <c r="Q113" s="1"/>
-    </row>
-    <row r="114" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M114" s="1"/>
-      <c r="N114" s="1"/>
-      <c r="O114" s="1"/>
-      <c r="P114" s="1"/>
-      <c r="Q114" s="1"/>
-    </row>
-    <row r="115" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B112" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C112" s="1">
+        <v>5</v>
+      </c>
+      <c r="D112" s="1">
+        <v>26</v>
+      </c>
+      <c r="E112" s="1">
+        <v>1</v>
+      </c>
+      <c r="F112" s="1">
+        <v>0</v>
+      </c>
+      <c r="G112" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H112" s="1">
+        <v>0</v>
+      </c>
+      <c r="I112" s="1">
+        <v>0</v>
+      </c>
+      <c r="J112" s="1">
+        <v>0</v>
+      </c>
+      <c r="K112" s="1">
+        <v>1</v>
+      </c>
+      <c r="L112" s="1">
+        <v>0</v>
+      </c>
+      <c r="M112" s="1">
+        <v>0</v>
+      </c>
+      <c r="N112" s="1">
+        <v>0</v>
+      </c>
+      <c r="O112" s="1">
+        <v>0</v>
+      </c>
+      <c r="P112" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B113" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C113" s="1">
+        <v>5</v>
+      </c>
+      <c r="D113" s="1">
+        <v>28</v>
+      </c>
+      <c r="E113" s="1">
+        <v>1</v>
+      </c>
+      <c r="F113" s="1">
+        <v>0</v>
+      </c>
+      <c r="G113" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H113" s="1">
+        <v>0</v>
+      </c>
+      <c r="I113" s="1">
+        <v>0</v>
+      </c>
+      <c r="J113" s="1">
+        <v>0</v>
+      </c>
+      <c r="K113" s="1">
+        <v>0</v>
+      </c>
+      <c r="L113" s="1">
+        <v>0</v>
+      </c>
+      <c r="M113" s="1">
+        <v>0</v>
+      </c>
+      <c r="N113" s="1">
+        <v>0</v>
+      </c>
+      <c r="O113" s="1">
+        <v>0</v>
+      </c>
+      <c r="P113" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q113" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B114" s="1">
+        <v>2025</v>
+      </c>
+      <c r="C114" s="1">
+        <v>6</v>
+      </c>
+      <c r="D114" s="1">
+        <v>8</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0</v>
+      </c>
+      <c r="F114" s="1">
+        <v>2</v>
+      </c>
+      <c r="G114" s="1">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H114" s="1">
+        <v>0</v>
+      </c>
+      <c r="I114" s="1">
+        <v>0</v>
+      </c>
+      <c r="J114" s="1">
+        <v>0</v>
+      </c>
+      <c r="K114" s="1">
+        <v>0</v>
+      </c>
+      <c r="L114" s="1">
+        <v>0</v>
+      </c>
+      <c r="M114" s="1">
+        <v>0</v>
+      </c>
+      <c r="N114" s="1">
+        <v>0</v>
+      </c>
+      <c r="O114" s="1">
+        <v>0</v>
+      </c>
+      <c r="P114" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q114" s="1">
+        <v>0</v>
+      </c>
+      <c r="R114" s="1"/>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
       <c r="O115" s="1"/>
       <c r="P115" s="1"/>
       <c r="Q115" s="1"/>
     </row>
-    <row r="116" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
       <c r="O116" s="1"/>
       <c r="P116" s="1"/>
       <c r="Q116" s="1"/>
     </row>
-    <row r="117" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
       <c r="O117" s="1"/>
       <c r="P117" s="1"/>
       <c r="Q117" s="1"/>
     </row>
-    <row r="118" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M118" s="1"/>
       <c r="N118" s="1"/>
       <c r="O118" s="1"/>
       <c r="P118" s="1"/>
       <c r="Q118" s="1"/>
     </row>
-    <row r="119" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
       <c r="O119" s="1"/>
       <c r="P119" s="1"/>
       <c r="Q119" s="1"/>
     </row>
-    <row r="120" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
       <c r="O120" s="1"/>
       <c r="P120" s="1"/>
       <c r="Q120" s="1"/>
     </row>
-    <row r="121" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M121" s="1"/>
       <c r="N121" s="1"/>
       <c r="O121" s="1"/>
       <c r="P121" s="1"/>
       <c r="Q121" s="1"/>
     </row>
-    <row r="122" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M122" s="1"/>
       <c r="N122" s="1"/>
       <c r="O122" s="1"/>
       <c r="P122" s="1"/>
       <c r="Q122" s="1"/>
     </row>
-    <row r="123" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
       <c r="O123" s="1"/>
       <c r="P123" s="1"/>
       <c r="Q123" s="1"/>
     </row>
-    <row r="124" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
       <c r="O124" s="1"/>
       <c r="P124" s="1"/>
       <c r="Q124" s="1"/>
     </row>
-    <row r="125" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
       <c r="O125" s="1"/>
       <c r="P125" s="1"/>
       <c r="Q125" s="1"/>
     </row>
-    <row r="126" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
       <c r="O126" s="1"/>
       <c r="P126" s="1"/>
       <c r="Q126" s="1"/>
     </row>
-    <row r="127" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
       <c r="O127" s="1"/>
       <c r="P127" s="1"/>
       <c r="Q127" s="1"/>
     </row>
-    <row r="128" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
       <c r="O128" s="1"/>

</xml_diff>